<commit_message>
removed the adminpage conflict and updated trackordertest page
</commit_message>
<xml_diff>
--- a/productData.xlsx
+++ b/productData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="44">
   <si>
     <t>imgsrc</t>
   </si>
@@ -35,13 +35,7 @@
     <t>http://localhost//shopping/product-details.php?pid=1</t>
   </si>
   <si>
-    <t>Micromax 81cm (32) HD Ready LED TV (32T6175MHD, 2 x HDMI, 2 x USB)</t>
-  </si>
-  <si>
-    <t>Rs.139900</t>
-  </si>
-  <si>
-    <t>Rs.0</t>
+    <t>null</t>
   </si>
   <si>
     <t>http://localhost//shopping/admin/productimages/2/apple-iphone-6-1.jpeg</t>
@@ -50,43 +44,28 @@
     <t>http://localhost//shopping/product-details.php?pid=2</t>
   </si>
   <si>
-    <t>Apple iPhone 6 (Silver, 16 GB)</t>
-  </si>
-  <si>
     <t>http://localhost//shopping/admin/productimages/3/mi-redmi-note-4-1.jpeg</t>
   </si>
   <si>
     <t>http://localhost//shopping/product-details.php?pid=3</t>
   </si>
   <si>
-    <t>Redmi Note 4 (Gold, 32 GB) (With 3 GB RAM)</t>
-  </si>
-  <si>
     <t>http://localhost//shopping/admin/productimages/4/lenovo-k6-power-k33a42-1.jpeg</t>
   </si>
   <si>
     <t>http://localhost//shopping/product-details.php?pid=4</t>
   </si>
   <si>
-    <t>Lenovo K6 Power (Silver, 32 GB)</t>
-  </si>
-  <si>
     <t>http://localhost//shopping/admin/productimages/5/lenovo-k5-note-pa330010in-1.jpeg</t>
   </si>
   <si>
     <t>http://localhost//shopping/product-details.php?pid=5</t>
   </si>
   <si>
-    <t>Lenovo Vibe K5 Note (Gold, 32 GB)</t>
-  </si>
-  <si>
     <t>http://localhost//shopping/admin/productimages/6/micromax-canvas-mega-4g-1.jpeg</t>
   </si>
   <si>
     <t>http://localhost//shopping/product-details.php?pid=6</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>http://localhost//shopping/admin/productimages/7/samsung-galaxy-on7-sm-1.jpeg</t>
@@ -243,316 +222,316 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>